<commit_message>
Avance Req 1 ordenamientos recursivos – Reto 1
</commit_message>
<xml_diff>
--- a/Docs/Maquina 1 ISIS1225 - Tablas de Datos Lab 4-5.xlsx
+++ b/Docs/Maquina 1 ISIS1225 - Tablas de Datos Lab 4-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/ESTRUCTURA DE DATOS/LABORATORIOS/Reto1-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AEBD3D18-DBCC-494B-9E1B-9D93992A8FC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16858893-9BD4-9641-9090-558D7F1E655A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="1" activeTab="6" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="2240" yWindow="820" windowWidth="24600" windowHeight="15580" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -92,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -155,61 +152,20 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -498,6 +454,56 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -637,7 +643,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -724,7 +730,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -772,37 +778,25 @@
             <c:numRef>
               <c:f>'Datos Lab4-5'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>2293.0100000000002</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>9248.66</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>38467.51</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>164240.64000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>688699.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -892,7 +886,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -943,34 +937,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>645.57000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2593.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10749.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>45474.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>190602.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>749434.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,7 +1041,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1103,7 +1085,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1153,35 +1135,32 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>77.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>171.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>417.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2158.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5339.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12081.23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>31470.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,7 +1257,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1329,34 +1308,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>29.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>58.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>118.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>546.61</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1124.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>2386.79</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>5017.01</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>11219.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,7 +1429,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1504,34 +1480,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>28.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>77.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>113.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>239.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>523.38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>1111.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>2392.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>5038.6899999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>10944.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1631,7 +1604,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1669,7 +1642,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1753,11 +1726,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1791,7 +1764,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1833,7 +1806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1870,7 +1843,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1946,7 +1919,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2043,7 +2016,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2094,34 +2067,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>44019.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2996884.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2210,7 +2162,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2261,34 +2213,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>321500.03999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2615806.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2377,7 +2308,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2428,34 +2359,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10308.120000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>48337.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1075527.6100000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,7 +2468,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2603,34 +2519,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>1683.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>8180.27</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>35358.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>184296.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>665179.06999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2727,7 +2628,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2775,37 +2676,28 @@
             <c:numRef>
               <c:f>'Datos Lab4-5'!$F$15:$F$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>215.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>837.87</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>3349.79</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>13507.21</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>55518.55</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>221963.72</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>900275.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2905,7 +2797,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2943,7 +2835,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -3027,7 +2919,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3065,7 +2957,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -3107,7 +2999,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3144,7 +3036,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3220,7 +3112,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3307,7 +3199,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3355,37 +3247,25 @@
             <c:numRef>
               <c:f>'Datos Lab4-5'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>2293.0100000000002</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>9248.66</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>38467.51</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>164240.64000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>688699.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3474,7 +3354,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3525,34 +3405,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>44019.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2996884.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3652,7 +3511,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3690,7 +3549,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3769,11 +3628,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3807,7 +3666,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3849,7 +3708,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3886,7 +3745,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3957,7 +3816,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4044,7 +3903,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4095,34 +3954,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>645.57000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2593.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10749.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>45474.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>190602.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>749434.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4211,7 +4058,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4262,34 +4109,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>321500.03999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2615806.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4389,7 +4215,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4427,7 +4253,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4506,7 +4332,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4544,7 +4370,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4586,7 +4412,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4623,7 +4449,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -4694,7 +4520,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4781,7 +4607,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4831,35 +4657,32 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>77.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>171.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>417.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2158.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5339.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12081.23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>31470.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4948,7 +4771,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4999,34 +4822,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10308.120000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>48337.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1075527.6100000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5126,7 +4934,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5164,7 +4972,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5243,11 +5051,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5281,7 +5089,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -5323,7 +5131,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5360,7 +5168,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -5439,7 +5247,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5526,7 +5334,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5577,34 +5385,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>29.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>58.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>118.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>546.61</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1124.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>2386.79</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>5017.01</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>11219.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5693,7 +5498,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5744,34 +5549,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>1683.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>8180.27</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>35358.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>184296.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>300</c:v>
+                  <c:v>665179.06999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5871,7 +5661,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5909,7 +5699,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5988,7 +5778,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6026,7 +5816,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -6068,7 +5858,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6105,7 +5895,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -6184,7 +5974,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6272,7 +6062,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6323,34 +6113,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>28.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>77.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>113.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>239.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>523.38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>1111.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>2392.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>5038.6899999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>330</c:v>
+                  <c:v>10944.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6440,7 +6227,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6488,37 +6275,28 @@
             <c:numRef>
               <c:f>'Datos Lab4-5'!$F$15:$F$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>215.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250</c:v>
+                  <c:v>837.87</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>3349.79</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>13507.21</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>55518.55</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>221963.72</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>900275.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6618,7 +6396,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6656,7 +6434,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -6735,7 +6513,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6773,7 +6551,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -6815,7 +6593,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6852,7 +6630,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -10759,7 +10537,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10770,7 +10548,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10781,7 +10559,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10792,7 +10570,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10803,7 +10581,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10814,7 +10592,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10825,7 +10603,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661400" cy="6286500"/>
+    <xdr:ext cx="8674100" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10858,7 +10636,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10891,7 +10669,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10924,7 +10702,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10957,7 +10735,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10990,7 +10768,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11023,7 +10801,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11060,21 +10838,21 @@
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Quick Sort [ms]" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{21628D13-D0BA-41D1-8E51-AB02437FBDE5}" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
@@ -11381,20 +11159,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22.1171875" customWidth="1"/>
+    <col min="5" max="6" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -11414,224 +11192,185 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4">
-        <v>15.7</v>
+      <c r="B2" s="6">
+        <v>563.12</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>645.57000000000005</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="D2" s="7">
+        <v>36.700000000000003</v>
       </c>
       <c r="E2" s="5">
-        <v>20</v>
+        <v>29.39</v>
       </c>
       <c r="F2" s="5">
-        <v>60</v>
+        <v>28.74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4">
-        <v>30</v>
+      <c r="B3" s="8">
+        <v>2293.0100000000002</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>2593.0700000000002</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>77.56</v>
       </c>
       <c r="E3" s="5">
-        <v>40</v>
+        <v>58.77</v>
       </c>
       <c r="F3" s="5">
-        <v>90</v>
+        <v>77.22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>45</v>
+        <v>9248.66</v>
       </c>
       <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>10749.37</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>171.08</v>
       </c>
       <c r="E4" s="5">
-        <v>60</v>
+        <v>118.51</v>
       </c>
       <c r="F4" s="5">
-        <v>120</v>
+        <v>113.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>60</v>
+        <v>38467.51</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>45474.61</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>417.92</v>
       </c>
       <c r="E5" s="5">
-        <v>80</v>
+        <v>295.14999999999998</v>
       </c>
       <c r="F5" s="5">
-        <v>150</v>
+        <v>239.77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>75</v>
+        <v>164240.64000000001</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>190602.47</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>913.15</v>
       </c>
       <c r="E6" s="5">
-        <v>100</v>
+        <v>546.61</v>
       </c>
       <c r="F6" s="5">
-        <v>180</v>
+        <v>523.38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4">
-        <v>90</v>
+        <v>688699.79</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>749434.38</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>2158.0700000000002</v>
       </c>
-      <c r="E7" s="5">
-        <v>120</v>
+      <c r="E7" s="8">
+        <v>1124.42</v>
       </c>
       <c r="F7" s="5">
-        <v>210</v>
+        <v>1111.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>105</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+        <v>5339.5</v>
       </c>
       <c r="E8" s="5">
-        <v>140</v>
+        <v>2386.79</v>
       </c>
       <c r="F8" s="5">
-        <v>240</v>
+        <v>2392.3000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>120</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <v>12081.23</v>
       </c>
       <c r="E9" s="5">
-        <v>160</v>
+        <v>5017.01</v>
       </c>
       <c r="F9" s="5">
-        <v>270</v>
+        <v>5038.6899999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>135</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>31470.36</v>
       </c>
       <c r="E10" s="5">
-        <v>180</v>
+        <v>11219.67</v>
       </c>
       <c r="F10" s="5">
-        <v>300</v>
+        <v>10944.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>150</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="E11" s="5">
-        <v>200</v>
-      </c>
-      <c r="F11" s="5">
-        <v>330</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -11651,222 +11390,151 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
       <c r="B15" s="4">
-        <v>50</v>
+        <v>44019.46</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>39137.78</v>
       </c>
       <c r="D15" s="4">
-        <v>35</v>
+        <v>2196.17</v>
       </c>
       <c r="E15" s="5">
-        <v>30</v>
+        <v>1683.83</v>
       </c>
       <c r="F15" s="5">
-        <v>70</v>
+        <v>215.55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
       <c r="B16" s="4">
-        <v>60</v>
+        <v>362439.99</v>
       </c>
       <c r="C16" s="4">
-        <v>4</v>
+        <v>321500.03999999998</v>
       </c>
       <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+        <v>10308.120000000001</v>
       </c>
       <c r="E16" s="5">
-        <v>60</v>
+        <v>8180.27</v>
       </c>
-      <c r="F16" s="5">
-        <v>90</v>
+      <c r="F16" s="8">
+        <v>837.87</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
       <c r="B17" s="4">
-        <v>70</v>
+        <v>2996884.79</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+        <v>2615806.89</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+        <v>48337.59</v>
       </c>
-      <c r="E17" s="5">
-        <v>90</v>
+      <c r="E17" s="6">
+        <v>35358.61</v>
       </c>
       <c r="F17" s="5">
-        <v>110</v>
+        <v>3349.79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <v>241678.25</v>
       </c>
       <c r="E18" s="5">
-        <v>120</v>
+        <v>184296.38</v>
       </c>
       <c r="F18" s="5">
-        <v>130</v>
+        <v>13507.21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <v>1075527.6100000001</v>
       </c>
       <c r="E19" s="5">
-        <v>150</v>
+        <v>665179.06999999995</v>
       </c>
       <c r="F19" s="5">
-        <v>150</v>
+        <v>55518.55</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
-      <c r="E20" s="5">
-        <v>180</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5">
-        <v>170</v>
+        <v>221963.72</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
-      <c r="E21" s="5">
-        <v>210</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="5">
-        <v>190</v>
+        <v>900275.62</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
-      <c r="E22" s="5">
-        <v>240</v>
-      </c>
-      <c r="F22" s="5">
-        <v>210</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
-      <c r="E23" s="5">
-        <v>270</v>
-      </c>
-      <c r="F23" s="5">
-        <v>230</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
-      <c r="E24" s="5">
-        <v>300</v>
-      </c>
-      <c r="F24" s="5">
-        <v>250</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11878,6 +11546,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c10596efcc8303131ba000bf7988b65d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88645b4f568d2e9f6d2a1da3b5a5f323" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -12088,34 +11771,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EE155A0-3C6B-4FBA-920A-A0416B6AA614}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -12130,4 +11786,31 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EE155A0-3C6B-4FBA-920A-A0416B6AA614}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Avance Req 1 ordenamientos iterativos – Reto 1
</commit_message>
<xml_diff>
--- a/Docs/Maquina 1 ISIS1225 - Tablas de Datos Lab 4-5.xlsx
+++ b/Docs/Maquina 1 ISIS1225 - Tablas de Datos Lab 4-5.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/ESTRUCTURA DE DATOS/LABORATORIOS/Reto1-G07/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianadiaz/Downloads/RETO 1/Reto1-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FF871-C8C8-7E43-8181-5F7ECCF2E9CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="820" windowWidth="24600" windowHeight="15580" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -22,9 +21,15 @@
     <sheet name="Graf Quick Sort" sheetId="11" r:id="rId7"/>
     <sheet name="Graf Merge Sort" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -82,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,9 +579,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -607,7 +612,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-419" sz="1800" b="1">
+              <a:rPr lang="x-none" sz="1800" b="1">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Comparación de rendimiento ARRAYLIST</a:t>
@@ -618,6 +623,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -643,7 +649,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -701,10 +707,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -730,7 +738,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -742,34 +750,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,7 +792,7 @@
                   <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2293.0100000000002</c:v>
+                  <c:v>2293.01</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
                   <c:v>9248.66</c:v>
@@ -793,7 +801,7 @@
                   <c:v>38467.51</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>164240.64000000001</c:v>
+                  <c:v>164240.64</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>688699.79</c:v>
@@ -802,7 +810,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EA19-4908-9336-CD0E2C6ECFDA}"/>
             </c:ext>
@@ -861,6 +869,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0933671504824708"/>
+                  <c:y val="0.107647021395053"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -886,7 +900,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -898,34 +912,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,10 +951,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>645.57000000000005</c:v>
+                  <c:v>645.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2593.0700000000002</c:v>
+                  <c:v>2593.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10749.37</c:v>
@@ -958,7 +972,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EA19-4908-9336-CD0E2C6ECFDA}"/>
             </c:ext>
@@ -1012,10 +1026,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0330231378471542"/>
+                  <c:y val="-0.00782613536944245"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1041,7 +1062,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1056,39 +1077,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1097,34 +1088,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,7 +1127,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>36.700000000000003</c:v>
+                  <c:v>36.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>77.56</c:v>
@@ -1151,7 +1142,7 @@
                   <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2158.0700000000002</c:v>
+                  <c:v>2158.07</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5339.5</c:v>
@@ -1166,7 +1157,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EA19-4908-9336-CD0E2C6ECFDA}"/>
             </c:ext>
@@ -1228,10 +1219,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0732940593260396"/>
+                  <c:y val="0.0651138153185397"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1257,7 +1254,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1269,34 +1266,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1317,7 +1314,7 @@
                   <c:v>118.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295.14999999999998</c:v>
+                  <c:v>295.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>546.61</c:v>
@@ -1338,7 +1335,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-0662-4A10-BB27-BF2CF30161F7}"/>
             </c:ext>
@@ -1400,10 +1397,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0498679978326281"/>
+                  <c:y val="0.11794018929452"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1429,7 +1432,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1441,34 +1444,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1498,10 +1501,10 @@
                   <c:v>1111.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2392.3000000000002</c:v>
+                  <c:v>2392.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5038.6899999999996</c:v>
+                  <c:v>5038.69</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10944.9</c:v>
@@ -1510,7 +1513,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-0662-4A10-BB27-BF2CF30161F7}"/>
             </c:ext>
@@ -1524,12 +1527,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="696671312"/>
-        <c:axId val="1833162896"/>
+        <c:axId val="-1691123616"/>
+        <c:axId val="-1693224800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="696671312"/>
+        <c:axId val="-1691123616"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1579,6 +1583,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1604,7 +1609,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1642,16 +1647,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833162896"/>
+        <c:crossAx val="-1693224800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1833162896"/>
+        <c:axId val="-1693224800"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1701,6 +1707,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1726,7 +1733,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1764,10 +1771,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="696671312"/>
+        <c:crossAx val="-1691123616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1781,6 +1788,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1806,20 +1818,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1843,16 +1855,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1883,7 +1895,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-419" sz="1800" b="1">
+              <a:rPr lang="x-none" sz="1800" b="1">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Comparación de rendimiento LINKED_LIST</a:t>
@@ -1894,6 +1906,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1919,7 +1932,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1930,10 +1943,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.9618151636373419E-2"/>
-          <c:y val="8.477122488864576E-2"/>
-          <c:w val="0.87419688477936697"/>
-          <c:h val="0.71422440045225488"/>
+          <c:x val="0.0896181516363734"/>
+          <c:y val="0.0847712248886457"/>
+          <c:w val="0.874196884779367"/>
+          <c:h val="0.714224400452255"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1987,10 +2000,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2016,7 +2031,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2028,34 +2043,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2073,13 +2088,13 @@
                   <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2996884.79</c:v>
+                  <c:v>2.99688479E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E4D7-4455-A92B-E398EC107F76}"/>
             </c:ext>
@@ -2133,10 +2148,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0868336191333709"/>
+                  <c:y val="0.0586876875768445"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2162,7 +2184,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2174,34 +2196,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2216,16 +2238,16 @@
                   <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>321500.03999999998</c:v>
+                  <c:v>321500.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2615806.89</c:v>
+                  <c:v>2.61580689E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-E4D7-4455-A92B-E398EC107F76}"/>
             </c:ext>
@@ -2279,10 +2301,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0319358890708811"/>
+                  <c:y val="0.0558116683934131"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2308,7 +2336,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2320,34 +2348,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2362,7 +2390,7 @@
                   <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10308.120000000001</c:v>
+                  <c:v>10308.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>48337.59</c:v>
@@ -2371,13 +2399,13 @@
                   <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1075527.6100000001</c:v>
+                  <c:v>1.07552761E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-E4D7-4455-A92B-E398EC107F76}"/>
             </c:ext>
@@ -2439,10 +2467,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0530827449684516"/>
+                  <c:y val="0.061984839845331"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2468,7 +2502,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2480,34 +2514,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2531,13 +2565,13 @@
                   <c:v>184296.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>665179.06999999995</c:v>
+                  <c:v>665179.0699999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-4887-4C16-ABE6-B7E1FD14A4B0}"/>
             </c:ext>
@@ -2599,10 +2633,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0560144220042907"/>
+                  <c:y val="0.0940566618894763"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2628,7 +2668,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2640,34 +2680,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2703,7 +2743,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-4887-4C16-ABE6-B7E1FD14A4B0}"/>
             </c:ext>
@@ -2717,12 +2757,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="696671312"/>
-        <c:axId val="1833162896"/>
+        <c:axId val="-1687617712"/>
+        <c:axId val="-1687619872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="696671312"/>
+        <c:axId val="-1687617712"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2772,6 +2813,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2797,7 +2839,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2835,16 +2877,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833162896"/>
+        <c:crossAx val="-1687619872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1833162896"/>
+        <c:axId val="-1687619872"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2894,6 +2937,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2919,7 +2963,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2957,10 +3001,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="696671312"/>
+        <c:crossAx val="-1687617712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2974,6 +3018,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2999,20 +3044,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3036,16 +3081,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3087,6 +3132,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3112,7 +3158,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3170,10 +3216,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3199,7 +3247,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3211,34 +3259,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3253,7 +3301,7 @@
                   <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2293.0100000000002</c:v>
+                  <c:v>2293.01</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
                   <c:v>9248.66</c:v>
@@ -3262,7 +3310,7 @@
                   <c:v>38467.51</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>164240.64000000001</c:v>
+                  <c:v>164240.64</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>688699.79</c:v>
@@ -3271,7 +3319,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B3D4-4A09-BEFF-C643A08A798B}"/>
             </c:ext>
@@ -3325,10 +3373,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3354,7 +3404,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3366,34 +3416,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3411,13 +3461,13 @@
                   <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2996884.79</c:v>
+                  <c:v>2.99688479E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B3D4-4A09-BEFF-C643A08A798B}"/>
             </c:ext>
@@ -3431,12 +3481,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1328118000"/>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1692185952"/>
+        <c:axId val="-1772142112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1328118000"/>
+        <c:axId val="-1692185952"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3486,6 +3537,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3511,7 +3563,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3549,16 +3601,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328121328"/>
+        <c:crossAx val="-1772142112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1772142112"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3603,6 +3656,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3628,7 +3682,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3666,10 +3720,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328118000"/>
+        <c:crossAx val="-1692185952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3683,6 +3737,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3708,20 +3763,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3745,16 +3800,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3791,6 +3846,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3816,7 +3872,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3874,10 +3930,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0875928542334397"/>
+                  <c:y val="0.145314779082525"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3903,7 +3966,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3915,34 +3978,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3954,10 +4017,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>645.57000000000005</c:v>
+                  <c:v>645.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2593.0700000000002</c:v>
+                  <c:v>2593.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10749.37</c:v>
@@ -3975,7 +4038,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C8DB-422B-A57B-18A87EA382C0}"/>
             </c:ext>
@@ -4029,10 +4092,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0415869929569345"/>
+                  <c:y val="0.0382085599953161"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4058,7 +4128,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4070,34 +4140,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4112,16 +4182,16 @@
                   <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>321500.03999999998</c:v>
+                  <c:v>321500.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2615806.89</c:v>
+                  <c:v>2.61580689E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C8DB-422B-A57B-18A87EA382C0}"/>
             </c:ext>
@@ -4135,12 +4205,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1328118000"/>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1664971056"/>
+        <c:axId val="-1664967936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1328118000"/>
+        <c:axId val="-1664971056"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4190,6 +4261,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4215,7 +4287,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4253,16 +4325,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328121328"/>
+        <c:crossAx val="-1664967936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1664967936"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4307,6 +4380,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4332,7 +4406,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4370,10 +4444,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328118000"/>
+        <c:crossAx val="-1664971056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4387,6 +4461,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4412,20 +4487,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4449,16 +4524,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4495,6 +4570,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4520,7 +4596,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4578,10 +4654,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4607,7 +4684,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4619,34 +4696,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4658,7 +4735,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>36.700000000000003</c:v>
+                  <c:v>36.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>77.56</c:v>
@@ -4673,7 +4750,7 @@
                   <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2158.0700000000002</c:v>
+                  <c:v>2158.07</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5339.5</c:v>
@@ -4688,7 +4765,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1191-4146-AA68-44FCE3413D1D}"/>
             </c:ext>
@@ -4742,10 +4819,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4771,7 +4849,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4783,34 +4861,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4825,7 +4903,7 @@
                   <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10308.120000000001</c:v>
+                  <c:v>10308.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>48337.59</c:v>
@@ -4834,13 +4912,13 @@
                   <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1075527.6100000001</c:v>
+                  <c:v>1.07552761E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1191-4146-AA68-44FCE3413D1D}"/>
             </c:ext>
@@ -4854,12 +4932,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1328118000"/>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1692576928"/>
+        <c:axId val="-1692565632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1328118000"/>
+        <c:axId val="-1692576928"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4909,6 +4988,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4934,7 +5014,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4972,16 +5052,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328121328"/>
+        <c:crossAx val="-1692565632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1692565632"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5026,6 +5107,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5051,7 +5133,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5089,10 +5171,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328118000"/>
+        <c:crossAx val="-1692576928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5106,6 +5188,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5131,20 +5214,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5168,16 +5251,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5218,8 +5301,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30724686335834317"/>
-          <c:y val="1.2117376349489305E-2"/>
+          <c:x val="0.307246863358343"/>
+          <c:y val="0.0121173763494893"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5247,7 +5330,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5305,10 +5388,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5334,7 +5418,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5346,34 +5430,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5394,7 +5478,7 @@
                   <c:v>118.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295.14999999999998</c:v>
+                  <c:v>295.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>546.61</c:v>
@@ -5415,7 +5499,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BB02-4A8D-958C-AC52A378B2B6}"/>
             </c:ext>
@@ -5469,10 +5553,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5498,7 +5583,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5510,34 +5595,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5561,13 +5646,13 @@
                   <c:v>184296.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>665179.06999999995</c:v>
+                  <c:v>665179.0699999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BB02-4A8D-958C-AC52A378B2B6}"/>
             </c:ext>
@@ -5581,12 +5666,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1328118000"/>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1691843136"/>
+        <c:axId val="-1691840288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1328118000"/>
+        <c:axId val="-1691843136"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5636,6 +5722,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5661,7 +5748,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5699,16 +5786,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328121328"/>
+        <c:crossAx val="-1691840288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1691840288"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5753,6 +5841,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5778,7 +5867,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5816,10 +5905,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328118000"/>
+        <c:crossAx val="-1691843136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5833,6 +5922,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5858,20 +5948,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5895,16 +5985,16 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5945,8 +6035,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30724686335834317"/>
-          <c:y val="1.2117376349489305E-2"/>
+          <c:x val="0.307246863358343"/>
+          <c:y val="0.0121173763494893"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5974,7 +6064,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6032,11 +6122,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00478913682079016"/>
+                  <c:y val="-0.0442744992223277"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6062,7 +6157,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6074,34 +6169,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6131,10 +6226,10 @@
                   <c:v>1111.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2392.3000000000002</c:v>
+                  <c:v>2392.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5038.6899999999996</c:v>
+                  <c:v>5038.69</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10944.9</c:v>
@@ -6143,7 +6238,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-32BC-41BA-A5CC-1F1B9359C7C7}"/>
             </c:ext>
@@ -6197,11 +6292,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6227,7 +6322,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CO"/>
+                  <a:endParaRPr lang="es-ES_tradnl"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6239,34 +6334,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16000</c:v>
+                  <c:v>16000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32000</c:v>
+                  <c:v>32000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64000</c:v>
+                  <c:v>64000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128000</c:v>
+                  <c:v>128000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256000</c:v>
+                  <c:v>256000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>512000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6302,7 +6397,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-32BC-41BA-A5CC-1F1B9359C7C7}"/>
             </c:ext>
@@ -6316,12 +6411,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1328118000"/>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1560567616"/>
+        <c:axId val="-1560564224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1328118000"/>
+        <c:axId val="-1560567616"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6371,6 +6467,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6396,7 +6493,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6434,16 +6531,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328121328"/>
+        <c:crossAx val="-1560564224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328121328"/>
+        <c:axId val="-1560564224"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6488,6 +6586,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6513,7 +6612,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CO"/>
+              <a:endParaRPr lang="es-ES_tradnl"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6551,10 +6650,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CO"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328118000"/>
+        <c:crossAx val="-1560567616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6568,6 +6667,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6593,20 +6693,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CO"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6630,7 +6730,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CO"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -10523,7 +10623,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10534,10 +10634,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10545,10 +10645,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10556,10 +10656,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10567,10 +10667,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10578,10 +10678,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10589,10 +10689,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10609,7 +10709,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86A8C9-B823-4237-B971-35F9FC141626}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F86A8C9-B823-4237-B971-35F9FC141626}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10636,13 +10736,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F79FD9B3-1053-4105-BF53-EDCA2C102566}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F79FD9B3-1053-4105-BF53-EDCA2C102566}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10669,13 +10769,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E62ACB43-BF23-44E0-A2C1-1BE0D48E226C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E62ACB43-BF23-44E0-A2C1-1BE0D48E226C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10702,13 +10802,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD62A27-62EF-4A76-950F-A06EC21FDB46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CD62A27-62EF-4A76-950F-A06EC21FDB46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10735,13 +10835,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49C9A0CC-8523-4ADB-8134-5F68720F3C67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49C9A0CC-8523-4ADB-8134-5F68720F3C67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10768,13 +10868,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9BA942-AC23-41C7-B38E-D0CB98EC3604}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C9BA942-AC23-41C7-B38E-D0CB98EC3604}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10801,13 +10901,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6272696"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DBB29D8-2208-4D18-B420-87681137F8B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2DBB29D8-2208-4D18-B420-87681137F8B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10831,30 +10931,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="8"/>
+    <tableColumn id="1" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="13"/>
+    <tableColumn id="2" name="Insertion Sort [ms]" dataDxfId="12"/>
+    <tableColumn id="3" name="Selection Sort [ms]" dataDxfId="11"/>
+    <tableColumn id="4" name="Shell Sort [ms]" dataDxfId="10"/>
+    <tableColumn id="5" name="Quick Sort [ms]" dataDxfId="9"/>
+    <tableColumn id="6" name="Merge Sort [ms]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A14:F24"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Quick Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{21628D13-D0BA-41D1-8E51-AB02437FBDE5}" name="Merge Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="1" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="5"/>
+    <tableColumn id="2" name="Insertion Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="3" name="Selection Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="4" name="Shell Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="5" name="Quick Sort [ms]" dataDxfId="1"/>
+    <tableColumn id="6" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11156,14 +11256,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
@@ -11172,7 +11272,7 @@
     <col min="5" max="6" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -11192,7 +11292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -11212,7 +11312,7 @@
         <v>28.74</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -11232,7 +11332,7 @@
         <v>77.22</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
@@ -11252,7 +11352,7 @@
         <v>113.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
@@ -11272,7 +11372,7 @@
         <v>239.77</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
@@ -11292,7 +11392,7 @@
         <v>523.38</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
@@ -11312,7 +11412,7 @@
         <v>1111.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
@@ -11328,7 +11428,7 @@
         <v>2392.3000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
@@ -11344,7 +11444,7 @@
         <v>5038.6899999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
@@ -11360,7 +11460,7 @@
         <v>10944.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
@@ -11370,7 +11470,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="16">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -11390,7 +11490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -11410,7 +11510,7 @@
         <v>215.55</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -11430,7 +11530,7 @@
         <v>837.87</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -11450,7 +11550,7 @@
         <v>3349.79</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -11466,7 +11566,7 @@
         <v>13507.21</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
@@ -11482,7 +11582,7 @@
         <v>55518.55</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
@@ -11494,7 +11594,7 @@
         <v>221963.72</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
@@ -11506,7 +11606,7 @@
         <v>900275.62</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
@@ -11516,7 +11616,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
@@ -11526,7 +11626,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>512000</v>
       </c>

</xml_diff>